<commit_message>
Ändrat namn på testerna.
</commit_message>
<xml_diff>
--- a/Geometry.Tests.xlsx
+++ b/Geometry.Tests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="131">
   <si>
     <t>Projekt</t>
   </si>
@@ -84,7 +84,7 @@
 Area fungerar.</t>
   </si>
   <si>
-    <t>ST_AreaTest_ValidInput_01</t>
+    <t>ST_AreaTest_PositiveInput_01</t>
   </si>
   <si>
     <t>Ett positivt värde returnerar arean.</t>
@@ -101,13 +101,13 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>ST_AreaTest_ValidInput_02</t>
+    <t>ST_AreaTest_PositiveInput_02</t>
   </si>
   <si>
     <t>Side: 4</t>
   </si>
   <si>
-    <t>ST_AreaTest_InvalidInput_01</t>
+    <t>ST_AreaTest_NegativeInput_01</t>
   </si>
   <si>
     <t>Ett negativt värde returnerar 0.</t>
@@ -128,7 +128,7 @@
 Perimiter fungerar.</t>
   </si>
   <si>
-    <t>ST_PerimiterTest_ValidInput_01</t>
+    <t>ST_PerimiterTest_PositiveInput_01</t>
   </si>
   <si>
     <t>Ett positivt värde returnerar omkretsen.</t>
@@ -137,7 +137,7 @@
     <t>Side: 5</t>
   </si>
   <si>
-    <t>ST_PerimiterTest_ValidInput_02</t>
+    <t>ST_PerimiterTest_PositiveInput_02</t>
   </si>
   <si>
     <t xml:space="preserve">1 - Ett positivt värde anges som värdet för sidan av kvadraten.
@@ -148,7 +148,7 @@
     <t>Side: 2.5</t>
   </si>
   <si>
-    <t>ST_PerimiterTest_InvalidInput_01</t>
+    <t>ST_PerimiterTest_NegativeInput_01</t>
   </si>
   <si>
     <t xml:space="preserve">1 - Ett negativt värde anges som värdet för sidan av kvadraten.
@@ -165,10 +165,10 @@
     <t>RT_AreaTest</t>
   </si>
   <si>
-    <t>RT_AreaTest_ValidInput_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Ett positivt värde anges som värdet för sidan av rektangeln.
+    <t>RT_AreaTest_PositiveInput_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Positiva värden anges som värden för sidorns av rektangeln.
 2 - Arean räknas ut.
 3 - Värdet på arean jämförs med det förväntade resultatet. </t>
   </si>
@@ -177,17 +177,17 @@
 Width: 3</t>
   </si>
   <si>
-    <t>RT_AreaTest_ValidInput_02</t>
+    <t>RT_AreaTest_PositiveInput_02</t>
   </si>
   <si>
     <t>Height: 4.2
 Width: 8.6</t>
   </si>
   <si>
-    <t>RT_AreaTest_InvalidInput_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Ett negativt värde anges som värdet för sidan av rektangeln.
+    <t>RT_AreaTest_NegativeInput_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Negativa värden anges som värden för sidorns av rektangeln.
 2 - Arean räknas ut.
 3 - Värdet på arean jämförs med det förväntade resultatet. </t>
   </si>
@@ -196,7 +196,7 @@
 Width: 8</t>
   </si>
   <si>
-    <t>RT_AreaTest_InvalidInput_02</t>
+    <t>RT_AreaTest_NegativeInput_02</t>
   </si>
   <si>
     <t>Height: 4
@@ -206,30 +206,30 @@
     <t>RT_PerimiterTest</t>
   </si>
   <si>
-    <t>RT_PerimiterTest_ValidInput_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Ett positivt värde anges som värdet för sidan av rektangeln.
+    <t>RT_PerimiterTest_PositiveInput_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Positiva värden anges som värden för sidorns av rektangeln.
 2 - Omkretsen räknas ut.
 3 - Värdet på omkretsen jämförs med det förväntade resultatet. </t>
   </si>
   <si>
-    <t>RT_PerimiterTest_ValidInput_02</t>
+    <t>RT_PerimiterTest_PositiveInput_02</t>
   </si>
   <si>
     <t>Height: 2.5
 Width: 4.2</t>
   </si>
   <si>
-    <t>RT_PerimiterTest_InvalidInput_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Ett negativt värde anges som värdet för sidan av rektangeln.
+    <t>RT_PerimiterTest_NegativeInput_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Negativa värden anges som värden för sidorns av rektangeln.
 2 - Omkretsen räknas ut.
 3 - Värdet på omkretsen jämförs med det förväntade resultatet. </t>
   </si>
   <si>
-    <t>RT_PerimiterTest_InvalidInput_02</t>
+    <t>RT_PerimiterTest_NegativeInput_02</t>
   </si>
   <si>
     <t>Circle</t>
@@ -238,7 +238,7 @@
     <t>CT_AreaTest</t>
   </si>
   <si>
-    <t>CT_AreaTest_ValidInput_01</t>
+    <t>CT_AreaTest_PositiveInput_01</t>
   </si>
   <si>
     <t xml:space="preserve">1 - Ett positivt värde anges som värdet för sidan av cirkeln.
@@ -249,13 +249,13 @@
     <t>Radius: 3</t>
   </si>
   <si>
-    <t>CT_AreaTest_ValidInput_02</t>
+    <t>CT_AreaTest_PositiveInput_02</t>
   </si>
   <si>
     <t>Radius: 6.3</t>
   </si>
   <si>
-    <t>CT_AreaTest_InvalidInput_01</t>
+    <t>CT_AreaTest_NegativeInput_01</t>
   </si>
   <si>
     <t xml:space="preserve">1 - Ett negativt värde anges som värdet för sidan av cirkeln.
@@ -269,7 +269,7 @@
     <t>CT_PerimiterTest</t>
   </si>
   <si>
-    <t>CT_PerimiterTest_ValidInput_01</t>
+    <t>CT_PerimiterTest_PositiveInput_01</t>
   </si>
   <si>
     <t xml:space="preserve">1 - Ett positivt värde anges som värdet för sidan av cirkeln.
@@ -277,10 +277,10 @@
 3 - Värdet på omkretsen jämförs med det förväntade resultatet. </t>
   </si>
   <si>
-    <t>CT_PerimiterTest_ValidInput_02</t>
-  </si>
-  <si>
-    <t>CT_PerimiterTest_InvalidInput_01</t>
+    <t>CT_PerimiterTest_PositiveInput_02</t>
+  </si>
+  <si>
+    <t>CT_PerimiterTest_NegativeInput_01</t>
   </si>
   <si>
     <t xml:space="preserve">1 - Ett negativt värde anges som värdet för sidan av cirkeln.
@@ -297,28 +297,38 @@
     <t>TT_AreaTest</t>
   </si>
   <si>
-    <t>TT_AreaTest_ValidInput_01</t>
+    <t>TT_AreaTest_PositiveInput_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Positiva värden anges som värden för basen och höjden av rektangeln.
+2 - Arean räknas ut.
+3 - Värdet på arean jämförs med det förväntade resultatet. </t>
   </si>
   <si>
     <t>Base: 5
 Height: 12</t>
   </si>
   <si>
-    <t>TT_AreaTest_ValidInput_02</t>
+    <t>TT_AreaTest_PositiveInput_02</t>
   </si>
   <si>
     <t>Base: 2.3
 Height: 1.4</t>
   </si>
   <si>
-    <t>TT_AreaTest_InvalidInput_01</t>
+    <t>TT_AreaTest_NegativeInput_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Negativa värden anges som värden för basen och höjden av rektangeln.
+2 - Arean räknas ut.
+3 - Värdet på arean jämförs med det förväntade resultatet. </t>
   </si>
   <si>
     <t>Base: 10
 Height: -2</t>
   </si>
   <si>
-    <t>TT_AreaTest_InvalidInput_02</t>
+    <t>TT_AreaTest_NegativeInput_02</t>
   </si>
   <si>
     <t>Base: -23
@@ -328,19 +338,29 @@
     <t>TT_PerimiterTest</t>
   </si>
   <si>
-    <t>TT_PerimiterTest_ValidInput_01</t>
+    <t>TT_PerimiterTest_PositiveInput_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Ett positivt värde anges som värdet för basen av rektangeln.
+2 - Omkretsen räknas ut.
+3 - Värdet på omkretsen jämförs med det förväntade resultatet. </t>
   </si>
   <si>
     <t>Base: 5</t>
   </si>
   <si>
-    <t>TT_PerimiterTest_ValidInput_02</t>
+    <t>TT_PerimiterTest_PositiveInput_02</t>
   </si>
   <si>
     <t>Base: 2.3</t>
   </si>
   <si>
-    <t>TT_PerimiterTest_InvalidInput_01</t>
+    <t>TT_PerimiterTest_NegativeInput_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Ett negativt värde anges som värdet för basen av rektangeln.
+2 - Omkretsen räknas ut.
+3 - Värdet på omkretsen jämförs med det förväntade resultatet. </t>
   </si>
   <si>
     <t>Base: -14</t>
@@ -482,11 +502,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <name val="Arial"/>
     </font>
@@ -511,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -525,13 +545,16 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -541,10 +564,10 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
@@ -783,7 +806,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="17.57"/>
     <col customWidth="1" min="2" max="2" width="23.71"/>
-    <col customWidth="1" min="3" max="3" width="29.71"/>
+    <col customWidth="1" min="3" max="3" width="31.71"/>
     <col customWidth="1" min="4" max="4" width="34.43"/>
     <col customWidth="1" min="5" max="5" width="56.14"/>
     <col customWidth="1" min="6" max="6" width="15.86"/>
@@ -898,7 +921,7 @@
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -927,7 +950,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -956,7 +979,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -991,7 +1014,7 @@
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1020,7 +1043,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1049,7 +1072,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1078,13 +1101,13 @@
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18">
-      <c r="C18" s="5"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19">
-      <c r="C19" s="5"/>
+      <c r="C19" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1103,7 +1126,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="15.71"/>
     <col customWidth="1" min="2" max="2" width="21.57"/>
-    <col customWidth="1" min="3" max="3" width="29.86"/>
+    <col customWidth="1" min="3" max="3" width="31.86"/>
     <col customWidth="1" min="4" max="4" width="34.0"/>
     <col customWidth="1" min="5" max="5" width="54.14"/>
   </cols>
@@ -1201,13 +1224,13 @@
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1230,59 +1253,59 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="9">
         <v>36.12</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="9">
         <v>36.12</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="6" t="s">
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="3">
         <v>44305.0</v>
       </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
     </row>
     <row r="11">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1305,13 +1328,13 @@
       </c>
     </row>
     <row r="12">
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1340,13 +1363,13 @@
       <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1369,13 +1392,13 @@
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1398,13 +1421,13 @@
       </c>
     </row>
     <row r="15">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -1427,13 +1450,13 @@
       </c>
     </row>
     <row r="16">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -1472,7 +1495,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="15.71"/>
     <col customWidth="1" min="2" max="2" width="21.57"/>
-    <col customWidth="1" min="3" max="3" width="29.86"/>
+    <col customWidth="1" min="3" max="3" width="31.86"/>
     <col customWidth="1" min="4" max="4" width="34.0"/>
     <col customWidth="1" min="5" max="5" width="54.14"/>
   </cols>
@@ -1570,7 +1593,7 @@
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1599,53 +1622,53 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="12">
         <v>124.6898</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="12">
         <v>124.6898</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="6" t="s">
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="3">
         <v>44305.0</v>
       </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
     </row>
     <row r="11">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1680,7 +1703,7 @@
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1709,7 +1732,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1738,7 +1761,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1783,9 +1806,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="15.71"/>
     <col customWidth="1" min="2" max="2" width="21.57"/>
-    <col customWidth="1" min="3" max="3" width="29.86"/>
+    <col customWidth="1" min="3" max="3" width="31.57"/>
     <col customWidth="1" min="4" max="4" width="34.0"/>
-    <col customWidth="1" min="5" max="5" width="54.14"/>
+    <col customWidth="1" min="5" max="5" width="63.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1881,17 +1904,17 @@
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>47</v>
+      <c r="E9" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G9" s="2">
         <v>30.0</v>
@@ -1910,63 +1933,63 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>47</v>
+      <c r="E10" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="10">
+        <v>87</v>
+      </c>
+      <c r="G10" s="12">
         <v>1.61</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="12">
         <v>1.61</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="6" t="s">
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="3">
         <v>44305.0</v>
       </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
     </row>
     <row r="11">
-      <c r="C11" s="2" t="s">
-        <v>87</v>
+      <c r="C11" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>52</v>
+      <c r="E11" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G11" s="2">
         <v>0.0</v>
@@ -1985,17 +2008,17 @@
       </c>
     </row>
     <row r="12">
-      <c r="C12" s="2" t="s">
-        <v>89</v>
+      <c r="C12" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>52</v>
+      <c r="E12" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G12" s="2">
         <v>0.0</v>
@@ -2015,22 +2038,22 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>92</v>
+      <c r="C13" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>58</v>
+      <c r="E13" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G13" s="2">
         <v>15.0</v>
@@ -2049,17 +2072,17 @@
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="5" t="s">
-        <v>94</v>
+      <c r="C14" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>58</v>
+      <c r="E14" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G14" s="2">
         <v>6.9</v>
@@ -2078,17 +2101,17 @@
       </c>
     </row>
     <row r="15">
-      <c r="C15" s="5" t="s">
-        <v>96</v>
+      <c r="C15" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>62</v>
+      <c r="E15" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G15" s="2">
         <v>0.0</v>
@@ -2142,8 +2165,8 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>98</v>
+      <c r="B2" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3">
@@ -2217,28 +2240,28 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="A9" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="B9" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="11">
+      <c r="C9" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="5">
         <v>59.1496</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="5">
         <v>59.1496</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -2252,209 +2275,209 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="3">
+        <v>44305.0</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+    </row>
+    <row r="11">
+      <c r="C11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="3">
+        <v>44305.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="3">
+        <v>44305.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="H10" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="3">
-        <v>44305.0</v>
-      </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-    </row>
-    <row r="11">
-      <c r="C11" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="G13" s="5">
+        <v>69.7543</v>
+      </c>
+      <c r="H13" s="5">
+        <v>69.7543</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="3">
+        <v>44305.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="E14" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="3">
-        <v>44305.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="G14" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="3">
+        <v>44305.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="3">
-        <v>44305.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="E15" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="G15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="3">
+        <v>44305.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G13" s="11">
-        <v>69.7543</v>
-      </c>
-      <c r="H13" s="11">
-        <v>69.7543</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K13" s="3">
-        <v>44305.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G14" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="H14" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" s="3">
-        <v>44305.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="3">
-        <v>44305.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>126</v>
+      <c r="E16" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="G16" s="2">
         <v>0.0</v>

</xml_diff>